<commit_message>
QA and UPdate files in console\Networking
</commit_message>
<xml_diff>
--- a/console/Networking/iaas-network/componentsMixinsXlsx/acl/aclListSelect.xlsx
+++ b/console/Networking/iaas-network/componentsMixinsXlsx/acl/aclListSelect.xlsx
@@ -1,208 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\han\Desktop\京东云-返工\18. ACL国际化内容翻译确认\4. 确认后-柴玉梅\2. 客户确认后-上传Github版\ACL国际化内容翻译确认-CT-C-GTCOM Comment1106-R\acl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ch" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ch" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aclListSelect_i18nKey_1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>选择需要关联的ACL，每个子网只能关联一个网络ACL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aclListSelect_i18nKey_2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>创建时间</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aclListSelect_i18nKey_3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>无ACL数据</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aclListSelect_i18nKey_4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'获取acl列表数据成功</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Select ACL needing to be associated, each subnet only can associate one network ACL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Creation Time</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>No ACL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> data</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>‘Got ACL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> list data</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>aclListSelect_i18nKey_1</t>
+  </si>
+  <si>
+    <t>选择需要关联的ACL，每个子网只能关联一个网络ACL</t>
+  </si>
+  <si>
+    <t>Select ACL needing to be associated, each subnet only can associate one network ACL</t>
+  </si>
+  <si>
+    <t>aclListSelect_i18nKey_2</t>
+  </si>
+  <si>
+    <t>创建时间</t>
+  </si>
+  <si>
+    <t>Creation Time</t>
+  </si>
+  <si>
+    <t>aclListSelect_i18nKey_3</t>
+  </si>
+  <si>
+    <t>无ACL数据</t>
+  </si>
+  <si>
+    <t>No ACL data</t>
+  </si>
+  <si>
+    <t>aclListSelect_i18nKey_4</t>
+  </si>
+  <si>
+    <t>'获取acl列表数据成功</t>
+  </si>
+  <si>
+    <t>'Got ACL list data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -218,25 +98,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -561,20 +432,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.44140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="22.44140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="46.21875" customWidth="1"/>
-    <col min="3" max="3" width="69.21875" customWidth="1"/>
+    <col customWidth="1" max="2" min="2" style="1" width="46.21875"/>
+    <col customWidth="1" max="3" min="3" style="1" width="69.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,51 +457,44 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:B4" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="1200" orientation="portrait" paperSize="9" verticalDpi="1200"/>
 </worksheet>
 </file>
</xml_diff>